<commit_message>
add hooking and success probability
</commit_message>
<xml_diff>
--- a/product data(기획 데이터).xlsx
+++ b/product data(기획 데이터).xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nayoonv\game-uruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4026D6F0-B8E8-4F8B-B27A-D00D959A852D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36F75C9-5896-472F-8445-FBB27ECC2475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29070" yWindow="-15930" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
+    <workbookView xWindow="-21288" yWindow="324" windowWidth="16320" windowHeight="11580" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
   </bookViews>
   <sheets>
-    <sheet name="non item" sheetId="1" r:id="rId1"/>
-    <sheet name="item" sheetId="2" r:id="rId2"/>
+    <sheet name="non_preparations" sheetId="1" r:id="rId1"/>
+    <sheet name="preparations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="157">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,10 +53,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물고기 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fish_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,10 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>grade_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fish_grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,10 +125,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물고기 등급 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>물고기 등급 명칭</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>지역 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>지역 명칭</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -177,14 +161,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>출항 비용(won)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출항 시간(m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>출항 가능 레벨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -225,18 +201,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이템 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이템 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이템 지불 방식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이템 지불 금액</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,10 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>낚싯대 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>낚싯대 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -305,22 +269,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fishing_rod_grade_percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>낚싯대 등급 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>낚싯대 등급 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>낚싯대 등급 확률(장점 부각 확률)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fishing_rod_durability</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,10 +305,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>낚싯줄 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>낚싯줄 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -397,10 +345,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>릴 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>릴 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -417,10 +361,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>릴 등급 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reel_grade_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -437,10 +377,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>미끼 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fishing_bait_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -481,10 +417,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>미끼 등급 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>미끼 등급 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -493,18 +425,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fishing_bait_class_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fishing_bait_class_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fishing_bait_class_percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fishing_hook</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -521,10 +441,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>낚시 바늘 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>낚시 바늘 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,6 +458,210 @@
   </si>
   <si>
     <t>낚시 바늘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>preparations_upgrade_item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_bait_grade_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_bait_grade_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_rod_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯대 종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 지불 방식(게임 내 돈, 캐시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_rod_type_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯대 종류 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_rod_type_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯대 종류 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>훅킹 확률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제압 성공률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등장 확률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hooking_probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success_probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing_bait_grade_appearance_probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>appearance_probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weather_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온도(정상 온도 범위: 10~20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_direction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_direction_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍향 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯대 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯대 등급 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚싯줄 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴 등급 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미끼 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미끼 등급 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚시 바늘 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기 등급 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날씨 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_direction_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍향 이름(8방위)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍속(m/s, 강풍 기준: 14m/s 이상)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간(0~23시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출항 비용(won, 장소의 거리에 따라 출항비용이 달라진다. 멀수록 비쌈)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출항 시간(m, 장소의 거리에 따라 출항시간이 달라진다. 멀수록 오래걸림)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fish_map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역 id(pk)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기 id(pk)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기가 여러 장소에 있을 수 있고, 먼 장소일수록 희귀한 물고기도 있으며 물고기 씨알도 굵어지기 때문에</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조수간만차</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,7 +726,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -629,13 +749,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -658,6 +789,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -974,21 +1132,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3242E66-B909-433E-B55E-F4A11B1BEF69}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="18.3984375" customWidth="1"/>
-    <col min="3" max="3" width="29.296875" customWidth="1"/>
+    <col min="1" max="1" width="21.8984375" customWidth="1"/>
+    <col min="2" max="2" width="22.296875" customWidth="1"/>
+    <col min="3" max="3" width="62.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -1010,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1018,10 +1177,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1029,10 +1188,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1040,10 +1199,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1051,185 +1210,365 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="5">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="5">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
+        <v>7</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" s="5">
+        <v>2</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" s="3">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" s="3">
         <v>4</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="5">
+      <c r="B30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" s="3">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="5">
-        <v>6</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="5">
-        <v>7</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>37</v>
+      <c r="B31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" s="3">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" s="3">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" s="3">
+        <v>4</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" s="3">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" s="3">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" s="3">
+        <v>2</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1241,25 +1580,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFF3889-4DE1-4EDC-BE51-A4C2BB00F684}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.69921875" customWidth="1"/>
-    <col min="2" max="2" width="29.3984375" customWidth="1"/>
-    <col min="3" max="3" width="79" customWidth="1"/>
+    <col min="2" max="2" width="49.59765625" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -1278,10 +1617,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1289,10 +1628,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1300,10 +1639,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1311,10 +1650,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1322,18 +1661,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -1352,10 +1691,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -1363,18 +1702,18 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
@@ -1393,10 +1732,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -1404,10 +1743,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -1415,10 +1754,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
@@ -1426,10 +1765,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
@@ -1437,144 +1776,150 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="9">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
+      <c r="A22" s="9">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="9">
+        <v>8</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="3">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="3">
-        <v>3</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>70</v>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" s="3">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" t="s">
-        <v>108</v>
+      <c r="A27" s="9">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" s="9">
+        <v>2</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" s="3">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>79</v>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
@@ -1593,10 +1938,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
@@ -1604,10 +1949,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
@@ -1615,10 +1960,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
@@ -1626,233 +1971,362 @@
         <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" s="3">
+      <c r="A42" s="9">
         <v>5</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" s="9">
+        <v>6</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" s="3">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>95</v>
+      <c r="B46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" s="3">
         <v>3</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>125</v>
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3">
+        <v>4</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" s="3">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" s="3">
+        <v>1</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" s="3">
+        <v>2</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" s="3">
+        <v>3</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A61" s="3">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A62" s="3">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A63" s="3">
+        <v>3</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A67" s="3">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A68" s="3">
+        <v>2</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A69" s="3">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A71" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A73" s="3">
+        <v>1</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
+      <c r="C73" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A74" s="3">
+        <v>2</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A75" s="3">
+        <v>3</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A76" s="9">
+        <v>4</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A77" s="9">
+        <v>5</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" s="3">
-        <v>1</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="3">
-        <v>2</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" s="3">
-        <v>3</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" s="3">
-        <v>1</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" s="3">
-        <v>2</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A60" s="3">
-        <v>3</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A62" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A64" s="3">
-        <v>1</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A65" s="3">
-        <v>2</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A66" s="3">
-        <v>3</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>123</v>
+      <c r="B80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add non-preparation item table
</commit_message>
<xml_diff>
--- a/product data(기획 데이터).xlsx
+++ b/product data(기획 데이터).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nayoonv\game-uruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36F75C9-5896-472F-8445-FBB27ECC2475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1D7E7-BCEC-41E0-ACFC-564E3E4F7F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21288" yWindow="324" windowWidth="16320" windowHeight="11580" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
   </bookViews>
   <sheets>
     <sheet name="non_preparations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="167">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -461,10 +461,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>preparations_upgrade_item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fishing_bait_grade_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -645,14 +641,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>지역 id(pk)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물고기 id(pk)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>물고기가 여러 장소에 있을 수 있고, 먼 장소일수록 희귀한 물고기도 있으며 물고기 씨알도 굵어지기 때문에</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -661,7 +649,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조수간만차</t>
+    <t>조수간만</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tide_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tide_power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tide_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>썰물:0, 밀물: 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tide_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조수간만 시간(PK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일자(1~7)(PK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역 id(PK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기 id(PK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조류 세기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upgrade_item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upgrade_item_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업그레이드 부품 id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1132,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3242E66-B909-433E-B55E-F4A11B1BEF69}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1169,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1213,7 +1253,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -1240,7 +1280,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -1289,7 +1329,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -1333,7 +1373,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
@@ -1344,7 +1384,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -1365,10 +1405,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="C25" s="16"/>
     </row>
@@ -1391,7 +1431,7 @@
         <v>33</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
@@ -1402,7 +1442,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
@@ -1445,7 +1485,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
@@ -1464,10 +1504,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
@@ -1475,10 +1515,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
@@ -1486,10 +1526,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
@@ -1497,10 +1537,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
@@ -1508,15 +1548,15 @@
         <v>5</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
@@ -1535,10 +1575,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
@@ -1546,18 +1586,18 @@
         <v>2</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>155</v>
+      <c r="A46" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
@@ -1569,6 +1609,50 @@
       </c>
       <c r="C47" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" s="3">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" s="3">
+        <v>2</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" s="3">
+        <v>3</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" s="3">
+        <v>4</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1582,13 +1666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFF3889-4DE1-4EDC-BE51-A4C2BB00F684}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.69921875" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" customWidth="1"/>
     <col min="2" max="2" width="49.59765625" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
   </cols>
@@ -1620,7 +1704,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1642,7 +1726,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1735,7 +1819,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -1787,10 +1871,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
@@ -1798,10 +1882,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -1809,10 +1893,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
@@ -1822,10 +1906,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="C25" s="10"/>
     </row>
@@ -1845,10 +1929,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
@@ -1856,10 +1940,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
@@ -1889,7 +1973,7 @@
         <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
@@ -1941,7 +2025,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
@@ -1982,10 +2066,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
@@ -1993,10 +2077,10 @@
         <v>6</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
@@ -2026,7 +2110,7 @@
         <v>71</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
@@ -2048,7 +2132,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
@@ -2100,7 +2184,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
@@ -2152,7 +2236,7 @@
         <v>84</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
@@ -2171,10 +2255,10 @@
         <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.4">
@@ -2201,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
@@ -2212,7 +2296,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>95</v>
@@ -2223,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>96</v>
@@ -2256,7 +2340,7 @@
         <v>98</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.4">
@@ -2286,10 +2370,10 @@
         <v>4</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
@@ -2297,15 +2381,15 @@
         <v>5</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
@@ -2319,9 +2403,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>165</v>
+      </c>
+      <c r="C81" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>